<commit_message>
Actualizo Planificación.mpp, Capacitaciones e Investigaciones.xlsx y Plan de Riesgos.docx
</commit_message>
<xml_diff>
--- a/Documentacion/Capacitaciones - Investigaciones/Capacitaciones e Investigaciones.xlsx
+++ b/Documentacion/Capacitaciones - Investigaciones/Capacitaciones e Investigaciones.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\2014\5TO\PROYECTO FINAL\ProyectoF\trunk\Documentacion\Capacitaciones - Investigaciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flor\Documents\Proyecto Final\Documentacion\Capacitaciones - Investigaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>Capacitaciones/Investigaciones</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>Documentacion\Capacitaciones-investigación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se necesitó investigar este tema para crear las url únicas  para cada torneo, edicion, equipo, jugador. </t>
+  </si>
+  <si>
+    <t>URL Rewriting en ASP.NET</t>
+  </si>
+  <si>
+    <t>#Sprint 13</t>
+  </si>
+  <si>
+    <t>Link a info https://msdn.microsoft.com/en-us/library/ms972974.aspx</t>
   </si>
 </sst>
 </file>
@@ -222,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -264,6 +276,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="H8" sqref="A1:H8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,6 +830,32 @@
         <v>35</v>
       </c>
     </row>
+    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>